<commit_message>
Done Scripting SCD0278 - Penyelia Mengajukan Data Non Sales
</commit_message>
<xml_diff>
--- a/Lib_Repo_Excel/FileExcel_Digisales/SCD0278 - Penyelia mengajukan data Non Sales.xlsx
+++ b/Lib_Repo_Excel/FileExcel_Digisales/SCD0278 - Penyelia mengajukan data Non Sales.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\1427\Documents\BNI\DigiSales\Lib_Repo_Excel\FileExcel_Digisales\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EB535C3-293D-4FEF-8127-F63425822457}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8D0FB9B-21D4-47FC-8160-EBCE765B4683}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="30">
   <si>
     <t>RUN</t>
   </si>
@@ -68,16 +68,40 @@
     <t>TEXT3</t>
   </si>
   <si>
-    <t>CIF</t>
-  </si>
-  <si>
-    <t>9448808661</t>
-  </si>
-  <si>
     <t>DGS-293</t>
   </si>
   <si>
     <t>Penyelia mengajukan data Non Sales</t>
+  </si>
+  <si>
+    <t>Penyelia</t>
+  </si>
+  <si>
+    <t>Pemimpin Cabang</t>
+  </si>
+  <si>
+    <t>SIDEBAR_MENU</t>
+  </si>
+  <si>
+    <t>SIDEBAR_SUBMENU</t>
+  </si>
+  <si>
+    <t>SIDEBAR_SUBMENU_SUBMENU</t>
+  </si>
+  <si>
+    <t>TEXT4</t>
+  </si>
+  <si>
+    <t>Monitoring</t>
+  </si>
+  <si>
+    <t>Approval</t>
+  </si>
+  <si>
+    <t>Monitoring,Report</t>
+  </si>
+  <si>
+    <t>Cuti Sakit</t>
   </si>
   <si>
     <t xml:space="preserve"> -Login sebagai penyelia
@@ -86,39 +110,30 @@
  -Isi form
  -Klik save
  -Setelah berhasil save 
- -Kirim Usulan
- -Pemimpin Cabang Approve Setuju</t>
+ -Kirim Usulan</t>
   </si>
   <si>
     <t>•	Saat input data field NPP  Hanya dapat memilih Sales yang berada dalam kewenangan Penyelia tersebut
 •	Saat berhasil Input data status di monitoring “Pengajuan”
-•	Saat berhasil Kirim Usulan status approval di monitoring menjadi “Menunggu Approval”
-•	Saat pemimpin Cabang melakukan approve setuju status  approval  di monitoring menjadi “Disetujui”
+•	Saat berhasil Kirim Usulan status approval di monitoring menjadi “Menunggu Approval”</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> -Login sebagai pemimpin cabang
+ -Pilih menu approval di fitur non sales update
+ -Pemimpin Cabang Approve Setuju</t>
+  </si>
+  <si>
+    <t>Pemimpin Cabang melakukan approve setuju status  approval  di monitoring menjadi “Disetujui”</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> -Login sebagai penyelia
+ -Pilih menu monitoring di fitur non sales update
+ -Cek status approval
+ -Cek Data report yang telah di approve</t>
+  </si>
+  <si>
+    <t>•	Saat pemimpin Cabang telah melakukan approve setuju maka status  approval  di monitoring menjadi “Disetujui”
 •	Pada report Status Sales berubah</t>
-  </si>
-  <si>
-    <t>Penyelia</t>
-  </si>
-  <si>
-    <t>Pemimpin Cabang</t>
-  </si>
-  <si>
-    <t>SIDEBAR_MENU</t>
-  </si>
-  <si>
-    <t>SIDEBAR_SUBMENU</t>
-  </si>
-  <si>
-    <t>SIDEBAR_SUBMENU_SUBMENU</t>
-  </si>
-  <si>
-    <t>TEXT4</t>
-  </si>
-  <si>
-    <t>Monitoring</t>
-  </si>
-  <si>
-    <t>Approval</t>
   </si>
 </sst>
 </file>
@@ -202,9 +217,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -216,6 +228,9 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -526,8 +541,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0EAF5E5-8229-45B3-AC11-8AED029F52F4}">
   <dimension ref="A1:S6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="84" zoomScaleNormal="84" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="84" zoomScaleNormal="84" workbookViewId="0">
+      <selection activeCell="N4" sqref="N4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -540,11 +555,11 @@
     <col min="6" max="6" width="7.28515625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="13.28515625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.28515625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="18.5703125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="28.7109375" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="13.42578125" customWidth="1"/>
-    <col min="13" max="13" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="13.140625" customWidth="1"/>
     <col min="15" max="15" width="25" customWidth="1"/>
     <col min="16" max="16" width="6.140625" bestFit="1" customWidth="1"/>
@@ -579,13 +594,13 @@
         <v>7</v>
       </c>
       <c r="I1" t="s">
-        <v>20</v>
-      </c>
-      <c r="J1" s="15" t="s">
-        <v>21</v>
-      </c>
-      <c r="K1" s="15" t="s">
-        <v>22</v>
+        <v>16</v>
+      </c>
+      <c r="J1" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="K1" s="14" t="s">
+        <v>18</v>
       </c>
       <c r="L1" t="s">
         <v>8</v>
@@ -597,24 +612,24 @@
         <v>11</v>
       </c>
       <c r="O1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:19" ht="153" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:19" ht="102" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="12" t="s">
-        <v>14</v>
+      <c r="B2" s="11" t="s">
+        <v>12</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="F2" s="9">
         <v>32362</v>
@@ -623,42 +638,46 @@
         <v>9</v>
       </c>
       <c r="H2" s="7" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="I2" s="7" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="J2" s="7"/>
       <c r="K2" s="7"/>
-      <c r="L2" s="7">
+      <c r="L2" s="14">
         <v>55210</v>
       </c>
-      <c r="M2" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="N2" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="O2" s="13"/>
+      <c r="M2" s="16" t="str">
+        <f ca="1">TEXT(TODAY(),"yyyy-mm-dd")</f>
+        <v>2022-08-30</v>
+      </c>
+      <c r="N2" s="16" t="str">
+        <f ca="1">TEXT(TODAY()+2,"yyyy-mm-dd")</f>
+        <v>2022-09-01</v>
+      </c>
+      <c r="O2" s="12" t="s">
+        <v>23</v>
+      </c>
       <c r="P2" s="7"/>
       <c r="R2" s="7"/>
       <c r="S2" s="7"/>
     </row>
-    <row r="3" spans="1:19" ht="153" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:19" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="12" t="s">
-        <v>14</v>
+      <c r="B3" s="11" t="s">
+        <v>12</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>16</v>
+        <v>26</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="F3" s="9">
         <v>18839</v>
@@ -667,38 +686,32 @@
         <v>9</v>
       </c>
       <c r="H3" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="I3" s="16" t="s">
-        <v>25</v>
-      </c>
-      <c r="L3">
-        <v>9315565540</v>
-      </c>
-      <c r="M3" t="s">
-        <v>12</v>
-      </c>
-      <c r="N3">
-        <v>9166244046</v>
+        <v>15</v>
+      </c>
+      <c r="I3" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="L3" s="14">
+        <v>55210</v>
       </c>
       <c r="O3" s="1"/>
       <c r="P3" s="2"/>
     </row>
-    <row r="4" spans="1:19" ht="153" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:19" ht="51" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="12" t="s">
-        <v>14</v>
+      <c r="B4" s="11" t="s">
+        <v>12</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="E4" s="8" t="s">
-        <v>17</v>
+        <v>29</v>
       </c>
       <c r="F4" s="9">
         <v>32362</v>
@@ -707,20 +720,19 @@
         <v>9</v>
       </c>
       <c r="H4" s="7" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="I4" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="L4">
-        <v>9003982023</v>
-      </c>
-      <c r="M4" t="s">
-        <v>12</v>
-      </c>
-      <c r="N4" s="14">
-        <v>9448808661</v>
-      </c>
+        <v>22</v>
+      </c>
+      <c r="L4" s="14">
+        <v>55210</v>
+      </c>
+      <c r="M4" s="14" t="str">
+        <f ca="1">TEXT(TODAY(),"yyyy")</f>
+        <v>2022</v>
+      </c>
+      <c r="N4" s="13"/>
       <c r="O4" s="1"/>
       <c r="P4" s="3"/>
       <c r="Q4" s="2"/>

</xml_diff>

<commit_message>
Done Scripting SCD0279 - SCD0281
</commit_message>
<xml_diff>
--- a/Lib_Repo_Excel/FileExcel_Digisales/SCD0278 - Penyelia mengajukan data Non Sales.xlsx
+++ b/Lib_Repo_Excel/FileExcel_Digisales/SCD0278 - Penyelia mengajukan data Non Sales.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\1427\Documents\BNI\DigiSales\Lib_Repo_Excel\FileExcel_Digisales\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8D0FB9B-21D4-47FC-8160-EBCE765B4683}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F10CE87-BFAA-466B-ABC0-3D0725CDB174}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="32">
   <si>
     <t>RUN</t>
   </si>
@@ -134,6 +134,12 @@
   <si>
     <t>•	Saat pemimpin Cabang telah melakukan approve setuju maka status  approval  di monitoring menjadi “Disetujui”
 •	Pada report Status Sales berubah</t>
+  </si>
+  <si>
+    <t>TEXT5</t>
+  </si>
+  <si>
+    <t>TEXT6</t>
   </si>
 </sst>
 </file>
@@ -542,7 +548,7 @@
   <dimension ref="A1:S6"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="G1" zoomScale="84" zoomScaleNormal="84" workbookViewId="0">
-      <selection activeCell="N4" sqref="N4"/>
+      <selection activeCell="Q2" sqref="Q2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -561,7 +567,7 @@
     <col min="12" max="12" width="13.42578125" customWidth="1"/>
     <col min="13" max="13" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="13.140625" customWidth="1"/>
-    <col min="15" max="15" width="25" customWidth="1"/>
+    <col min="15" max="15" width="6.28515625" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="6.140625" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="23.42578125" customWidth="1"/>
     <col min="18" max="18" width="16.42578125" bestFit="1" customWidth="1"/>
@@ -614,8 +620,14 @@
       <c r="O1" t="s">
         <v>19</v>
       </c>
+      <c r="P1" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>31</v>
+      </c>
     </row>
-    <row r="2" spans="1:19" ht="102" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:19" ht="89.25" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>0</v>
       </c>
@@ -656,10 +668,10 @@
         <f ca="1">TEXT(TODAY()+2,"yyyy-mm-dd")</f>
         <v>2022-09-01</v>
       </c>
-      <c r="O2" s="12" t="s">
+      <c r="P2" s="7"/>
+      <c r="Q2" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="P2" s="7"/>
       <c r="R2" s="7"/>
       <c r="S2" s="7"/>
     </row>

</xml_diff>